<commit_message>
ex 10 in the books
</commit_message>
<xml_diff>
--- a/HW1/HW1_ex8.xlsx
+++ b/HW1/HW1_ex8.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10909"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F782FAFD-582F-8A4D-B391-D5D67E264EEB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B65D81-5664-6142-93F9-D63712200344}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="23720" windowHeight="14400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="460" windowWidth="23720" windowHeight="14400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment Problem_BEST" sheetId="10" r:id="rId1"/>
@@ -15,74 +15,106 @@
   <definedNames>
     <definedName name="OpenSolver_ChosenSolver" localSheetId="0" hidden="1">CBC</definedName>
     <definedName name="OpenSolver_ChosenSolver" localSheetId="1" hidden="1">CBC</definedName>
+    <definedName name="OpenSolver_ChosenSolver" localSheetId="2" hidden="1">CBC</definedName>
     <definedName name="OpenSolver_DualsNewSheet" localSheetId="0" hidden="1">0</definedName>
     <definedName name="OpenSolver_DualsNewSheet" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="OpenSolver_DualsNewSheet" localSheetId="2" hidden="1">0</definedName>
     <definedName name="OpenSolver_LinearityCheck" localSheetId="0" hidden="1">1</definedName>
     <definedName name="OpenSolver_LinearityCheck" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="OpenSolver_LinearityCheck" localSheetId="2" hidden="1">1</definedName>
     <definedName name="OpenSolver_UpdateSensitivity" localSheetId="0" hidden="1">1</definedName>
     <definedName name="OpenSolver_UpdateSensitivity" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="OpenSolver_UpdateSensitivity" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'Assignment Problem_BEST'!$D$21:$M$30</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">'Assignment Problem_WORST'!$D$21:$M$30</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">'Distributor Problem'!$H$5:$H$19</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Assignment Problem_BEST'!$N$21:$N$30</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Assignment Problem_WORST'!$N$21:$N$30</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">'Distributor Problem'!$H$5:$H$19</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Assignment Problem_BEST'!$D$31:$M$31</definedName>
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">'Assignment Problem_WORST'!$D$31:$M$31</definedName>
+    <definedName name="solver_lhs2" localSheetId="2" hidden="1">'Distributor Problem'!$H$5:$H$19</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Assignment Problem_BEST'!$D$21:$M$30</definedName>
     <definedName name="solver_lhs3" localSheetId="1" hidden="1">'Assignment Problem_WORST'!$D$21:$M$30</definedName>
+    <definedName name="solver_lhs3" localSheetId="2" hidden="1">'Distributor Problem'!$I$20</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">'Assignment Problem_BEST'!$D$21:$M$30</definedName>
     <definedName name="solver_lhs4" localSheetId="1" hidden="1">'Assignment Problem_WORST'!$D$21:$M$30</definedName>
+    <definedName name="solver_lhs4" localSheetId="2" hidden="1">'Distributor Problem'!$J$20</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_lin" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">4</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">4</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'Assignment Problem_BEST'!$N$31</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">'Assignment Problem_WORST'!$N$31</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">'Distributor Problem'!$L$21</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_rel3" localSheetId="1" hidden="1">4</definedName>
+    <definedName name="solver_rel3" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">'Distributor Problem'!$F$5:$F$19</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs2" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rhs2" localSheetId="2" hidden="1">'Distributor Problem'!$E$5:$E$19</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">integer</definedName>
     <definedName name="solver_rhs3" localSheetId="1" hidden="1">integer</definedName>
+    <definedName name="solver_rhs3" localSheetId="2" hidden="1">18000</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs4" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rhs4" localSheetId="2" hidden="1">30000</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">9999999999</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">9999999999</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.05</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.05</definedName>
+    <definedName name="solver_tol" localSheetId="2" hidden="1">0.05</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
   </definedNames>
@@ -91,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="41">
   <si>
     <t>Min</t>
   </si>
@@ -136,9 +168,6 @@
   </si>
   <si>
     <t>Profit Per Product</t>
-  </si>
-  <si>
-    <t>Vegtable</t>
   </si>
   <si>
     <t>Cost</t>
@@ -197,6 +226,27 @@
   <si>
     <t>Best Allocations</t>
   </si>
+  <si>
+    <t>TOTALS</t>
+  </si>
+  <si>
+    <t>Number of cartons</t>
+  </si>
+  <si>
+    <t>Cost per product</t>
+  </si>
+  <si>
+    <t>Revenue per product</t>
+  </si>
+  <si>
+    <t>PROFITS</t>
+  </si>
+  <si>
+    <t>Volume per product</t>
+  </si>
+  <si>
+    <t>Vegetable</t>
+  </si>
 </sst>
 </file>
 
@@ -205,7 +255,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,16 +278,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -414,14 +484,189 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -438,7 +683,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -448,6 +692,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -19687,6 +19950,1059 @@
               </a:solidFill>
             </a:rPr>
             <a:t>i</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="OpenSolver1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BB7E72C-FD55-9340-B814-2AFC53F6F5DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6070600" y="774700"/>
+          <a:ext cx="1143000" cy="2870200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF00FF">
+            <a:alpha val="40000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF00FF"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="OpenSolver2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B063B5B-26F9-C742-A3CC-5A47DFE0B402}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10998200" y="3848100"/>
+          <a:ext cx="673100" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="FF00FF"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF00FF"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>236535</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="OpenSolver3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9D40B4C-99F9-8A45-8B20-0CD804E073FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10985500" y="3771900"/>
+          <a:ext cx="249235" cy="127000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF">
+            <a:alpha val="80000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="12700" tIns="0" rIns="12700" bIns="0" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="900">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>max </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="OpenSolver4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24304188-F514-AB41-9452-DC81E412F13E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3937000" y="774700"/>
+          <a:ext cx="673100" cy="2870200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="0000FF"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="0000FF"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="OpenSolver5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{697DD743-2B24-104A-A151-18B2237EA5AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6083300" y="787400"/>
+          <a:ext cx="1130300" cy="2857500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="0000FF"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>≥</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="OpenSolver6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8ADFB2A3-527D-6841-9D24-0B4E2B1E1EA3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="3"/>
+          <a:endCxn id="6" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4610100" y="2209800"/>
+          <a:ext cx="1473200" cy="6350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:srgbClr val="0000FF"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:headEnd type="none"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>168275</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>927100</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>41275</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="OpenSolver7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD0589EB-70A9-D74F-A32E-8FF3A889FB7F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5156200" y="2085975"/>
+          <a:ext cx="381000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="OpenSolver8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68D78D7F-524D-0742-AA7E-E75B30491B9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3263900" y="774700"/>
+          <a:ext cx="673100" cy="2870200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="008000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="008000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="OpenSolver9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24CB6BFC-F983-C24F-A66E-D7D211D6916C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6096000" y="800100"/>
+          <a:ext cx="1117600" cy="2844800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="008000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="008000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>≤</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="OpenSolver10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDA50B3E-7E53-9D4B-BB91-B8244F217393}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="3"/>
+          <a:endCxn id="10" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3937000" y="2209800"/>
+          <a:ext cx="2159000" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:srgbClr val="008000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:headEnd type="none"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="OpenSolver11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8B97429-3255-684F-AF07-E34AB89B6703}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4826000" y="2089150"/>
+          <a:ext cx="381000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="OpenSolverI20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C2DEA94-F344-4545-9CC8-DBD96DDD7D97}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7213600" y="3644900"/>
+          <a:ext cx="1295400" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="9900CC"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="9900CC"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>18000≥</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="OpenSolverJ20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62F083B1-F413-3A45-BD4E-04A54DFA7655}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8509000" y="3644900"/>
+          <a:ext cx="1143000" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="800000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="800000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>30000≥</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -20033,502 +21349,502 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="21"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="19"/>
     </row>
     <row r="5" spans="3:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>2</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>3</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>4</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>5</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <v>6</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="2">
         <v>7</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="2">
         <v>8</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="2">
         <v>9</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>14</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>18</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>22</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <v>27</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="6">
         <v>23</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="6">
         <v>21</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="6">
         <v>27</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="6">
         <v>31</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="6">
         <v>20</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="7">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>22</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <v>20</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="10">
         <v>19</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="10">
         <v>19</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="10">
         <v>25</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="10">
         <v>19</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="10">
         <v>28</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="10">
         <v>20</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="10">
         <v>27</v>
       </c>
-      <c r="M7" s="12">
+      <c r="M7" s="11">
         <v>39</v>
       </c>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>12</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="10">
         <v>18</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <v>17</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="10">
         <v>16</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="10">
         <v>25</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="10">
         <v>30</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="10">
         <v>27</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="10">
         <v>26</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="10">
         <v>29</v>
       </c>
-      <c r="M8" s="12">
+      <c r="M8" s="11">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>12</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="10">
         <v>23</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="10">
         <v>26</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="10">
         <v>19</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="10">
         <v>26</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="10">
         <v>20</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="10">
         <v>26</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="10">
         <v>34</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="10">
         <v>23</v>
       </c>
-      <c r="M9" s="12">
+      <c r="M9" s="11">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>12</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="10">
         <v>14</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="10">
         <v>14</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="10">
         <v>19</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="10">
         <v>21</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="10">
         <v>27</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="10">
         <v>24</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="10">
         <v>28</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="10">
         <v>26</v>
       </c>
-      <c r="M10" s="12">
+      <c r="M10" s="11">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>20</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="10">
         <v>18</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="10">
         <v>20</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="10">
         <v>19</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="10">
         <v>15</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="10">
         <v>20</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="10">
         <v>31</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="10">
         <v>32</v>
       </c>
-      <c r="L11" s="11">
+      <c r="L11" s="10">
         <v>26</v>
       </c>
-      <c r="M11" s="12">
+      <c r="M11" s="11">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <v>15</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="10">
         <v>23</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="10">
         <v>20</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="10">
         <v>23</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="10">
         <v>26</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="10">
         <v>22</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="10">
         <v>32</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="10">
         <v>24</v>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="10">
         <v>26</v>
       </c>
-      <c r="M12" s="12">
+      <c r="M12" s="11">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <v>13</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="10">
         <v>14</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="10">
         <v>19</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="10">
         <v>20</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="10">
         <v>21</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="10">
         <v>22</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="10">
         <v>32</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="10">
         <v>24</v>
       </c>
-      <c r="L13" s="11">
+      <c r="L13" s="10">
         <v>31</v>
       </c>
-      <c r="M13" s="12">
+      <c r="M13" s="11">
         <v>29</v>
       </c>
     </row>
     <row r="14" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="9">
         <v>14</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="10">
         <v>19</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="10">
         <v>15</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="10">
         <v>16</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="10">
         <v>20</v>
       </c>
-      <c r="I14" s="11">
+      <c r="I14" s="10">
         <v>22</v>
       </c>
-      <c r="J14" s="11">
+      <c r="J14" s="10">
         <v>27</v>
       </c>
-      <c r="K14" s="11">
+      <c r="K14" s="10">
         <v>33</v>
       </c>
-      <c r="L14" s="11">
+      <c r="L14" s="10">
         <v>19</v>
       </c>
-      <c r="M14" s="12">
+      <c r="M14" s="11">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="3:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="13">
         <v>18</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="14">
         <v>23</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="14">
         <v>14</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G15" s="14">
         <v>23</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="14">
         <v>24</v>
       </c>
-      <c r="I15" s="15">
+      <c r="I15" s="14">
         <v>31</v>
       </c>
-      <c r="J15" s="15">
+      <c r="J15" s="14">
         <v>18</v>
       </c>
-      <c r="K15" s="15">
+      <c r="K15" s="14">
         <v>19</v>
       </c>
-      <c r="L15" s="15">
+      <c r="L15" s="14">
         <v>32</v>
       </c>
-      <c r="M15" s="16">
+      <c r="M15" s="15">
         <v>35</v>
       </c>
     </row>
     <row r="16" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
     </row>
     <row r="18" spans="3:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="3:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="21"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="19"/>
     </row>
     <row r="20" spans="3:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>1</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <v>2</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2">
         <v>3</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="2">
         <v>4</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="2">
         <v>5</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20" s="2">
         <v>6</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="2">
         <v>7</v>
       </c>
-      <c r="K20" s="3">
+      <c r="K20" s="2">
         <v>8</v>
       </c>
-      <c r="L20" s="3">
+      <c r="L20" s="2">
         <v>9</v>
       </c>
-      <c r="M20" s="4">
+      <c r="M20" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="5">
         <v>0</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="6">
         <v>0</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="6">
         <v>0</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="6">
         <v>1</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H21" s="6">
         <v>0</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="6">
         <v>0</v>
       </c>
-      <c r="J21" s="7">
+      <c r="J21" s="6">
         <v>0</v>
       </c>
-      <c r="K21" s="7">
+      <c r="K21" s="6">
         <v>0</v>
       </c>
-      <c r="L21" s="7">
+      <c r="L21" s="6">
         <v>0</v>
       </c>
-      <c r="M21" s="8">
+      <c r="M21" s="7">
         <v>0</v>
       </c>
       <c r="N21">
@@ -20537,37 +21853,37 @@
       </c>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="9">
         <v>0</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E22" s="10">
         <v>0</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="10">
         <v>0</v>
       </c>
-      <c r="G22" s="11">
+      <c r="G22" s="10">
         <v>0</v>
       </c>
-      <c r="H22" s="11">
+      <c r="H22" s="10">
         <v>0</v>
       </c>
-      <c r="I22" s="11">
+      <c r="I22" s="10">
         <v>0</v>
       </c>
-      <c r="J22" s="11">
+      <c r="J22" s="10">
         <v>0</v>
       </c>
-      <c r="K22" s="11">
+      <c r="K22" s="10">
         <v>0</v>
       </c>
-      <c r="L22" s="11">
+      <c r="L22" s="10">
         <v>0</v>
       </c>
-      <c r="M22" s="12">
+      <c r="M22" s="11">
         <v>1</v>
       </c>
       <c r="N22">
@@ -20576,37 +21892,37 @@
       </c>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="9">
         <v>0</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E23" s="10">
         <v>0</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="10">
         <v>0</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="10">
         <v>0</v>
       </c>
-      <c r="H23" s="11">
+      <c r="H23" s="10">
         <v>1</v>
       </c>
-      <c r="I23" s="11">
+      <c r="I23" s="10">
         <v>0</v>
       </c>
-      <c r="J23" s="11">
+      <c r="J23" s="10">
         <v>0</v>
       </c>
-      <c r="K23" s="11">
+      <c r="K23" s="10">
         <v>0</v>
       </c>
-      <c r="L23" s="11">
+      <c r="L23" s="10">
         <v>0</v>
       </c>
-      <c r="M23" s="12">
+      <c r="M23" s="11">
         <v>0</v>
       </c>
       <c r="N23">
@@ -20615,37 +21931,37 @@
       </c>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="9">
         <v>0</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="10">
         <v>0</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="10">
         <v>1</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G24" s="10">
         <v>0</v>
       </c>
-      <c r="H24" s="11">
+      <c r="H24" s="10">
         <v>0</v>
       </c>
-      <c r="I24" s="11">
+      <c r="I24" s="10">
         <v>0</v>
       </c>
-      <c r="J24" s="11">
+      <c r="J24" s="10">
         <v>0</v>
       </c>
-      <c r="K24" s="11">
+      <c r="K24" s="10">
         <v>0</v>
       </c>
-      <c r="L24" s="11">
+      <c r="L24" s="10">
         <v>0</v>
       </c>
-      <c r="M24" s="12">
+      <c r="M24" s="11">
         <v>0</v>
       </c>
       <c r="N24">
@@ -20654,37 +21970,37 @@
       </c>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="9">
         <v>0</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="10">
         <v>0</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="10">
         <v>0</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G25" s="10">
         <v>0</v>
       </c>
-      <c r="H25" s="11">
+      <c r="H25" s="10">
         <v>0</v>
       </c>
-      <c r="I25" s="11">
+      <c r="I25" s="10">
         <v>1</v>
       </c>
-      <c r="J25" s="11">
+      <c r="J25" s="10">
         <v>0</v>
       </c>
-      <c r="K25" s="11">
+      <c r="K25" s="10">
         <v>0</v>
       </c>
-      <c r="L25" s="11">
+      <c r="L25" s="10">
         <v>0</v>
       </c>
-      <c r="M25" s="12">
+      <c r="M25" s="11">
         <v>0</v>
       </c>
       <c r="N25">
@@ -20693,37 +22009,37 @@
       </c>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="9">
         <v>1</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26" s="10">
         <v>0</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="10">
         <v>0</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G26" s="10">
         <v>0</v>
       </c>
-      <c r="H26" s="11">
+      <c r="H26" s="10">
         <v>0</v>
       </c>
-      <c r="I26" s="11">
+      <c r="I26" s="10">
         <v>0</v>
       </c>
-      <c r="J26" s="11">
+      <c r="J26" s="10">
         <v>0</v>
       </c>
-      <c r="K26" s="11">
+      <c r="K26" s="10">
         <v>0</v>
       </c>
-      <c r="L26" s="11">
+      <c r="L26" s="10">
         <v>0</v>
       </c>
-      <c r="M26" s="12">
+      <c r="M26" s="11">
         <v>0</v>
       </c>
       <c r="N26">
@@ -20732,37 +22048,37 @@
       </c>
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27" s="9">
         <v>0</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E27" s="10">
         <v>1</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F27" s="10">
         <v>0</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G27" s="10">
         <v>0</v>
       </c>
-      <c r="H27" s="11">
+      <c r="H27" s="10">
         <v>0</v>
       </c>
-      <c r="I27" s="11">
+      <c r="I27" s="10">
         <v>0</v>
       </c>
-      <c r="J27" s="11">
+      <c r="J27" s="10">
         <v>0</v>
       </c>
-      <c r="K27" s="11">
+      <c r="K27" s="10">
         <v>0</v>
       </c>
-      <c r="L27" s="11">
+      <c r="L27" s="10">
         <v>0</v>
       </c>
-      <c r="M27" s="12">
+      <c r="M27" s="11">
         <v>0</v>
       </c>
       <c r="N27">
@@ -20771,37 +22087,37 @@
       </c>
     </row>
     <row r="28" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="9">
         <v>0</v>
       </c>
-      <c r="E28" s="11">
+      <c r="E28" s="10">
         <v>0</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F28" s="10">
         <v>0</v>
       </c>
-      <c r="G28" s="11">
+      <c r="G28" s="10">
         <v>0</v>
       </c>
-      <c r="H28" s="11">
+      <c r="H28" s="10">
         <v>0</v>
       </c>
-      <c r="I28" s="11">
+      <c r="I28" s="10">
         <v>0</v>
       </c>
-      <c r="J28" s="11">
+      <c r="J28" s="10">
         <v>1</v>
       </c>
-      <c r="K28" s="11">
+      <c r="K28" s="10">
         <v>0</v>
       </c>
-      <c r="L28" s="11">
+      <c r="L28" s="10">
         <v>0</v>
       </c>
-      <c r="M28" s="12">
+      <c r="M28" s="11">
         <v>0</v>
       </c>
       <c r="N28">
@@ -20810,37 +22126,37 @@
       </c>
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="9">
         <v>0</v>
       </c>
-      <c r="E29" s="11">
+      <c r="E29" s="10">
         <v>0</v>
       </c>
-      <c r="F29" s="11">
+      <c r="F29" s="10">
         <v>0</v>
       </c>
-      <c r="G29" s="11">
+      <c r="G29" s="10">
         <v>0</v>
       </c>
-      <c r="H29" s="11">
+      <c r="H29" s="10">
         <v>0</v>
       </c>
-      <c r="I29" s="11">
+      <c r="I29" s="10">
         <v>0</v>
       </c>
-      <c r="J29" s="11">
+      <c r="J29" s="10">
         <v>0</v>
       </c>
-      <c r="K29" s="11">
+      <c r="K29" s="10">
         <v>1</v>
       </c>
-      <c r="L29" s="11">
+      <c r="L29" s="10">
         <v>0</v>
       </c>
-      <c r="M29" s="12">
+      <c r="M29" s="11">
         <v>0</v>
       </c>
       <c r="N29">
@@ -20849,37 +22165,37 @@
       </c>
     </row>
     <row r="30" spans="3:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="14">
+      <c r="D30" s="13">
         <v>0</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="14">
         <v>0</v>
       </c>
-      <c r="F30" s="15">
+      <c r="F30" s="14">
         <v>0</v>
       </c>
-      <c r="G30" s="15">
+      <c r="G30" s="14">
         <v>0</v>
       </c>
-      <c r="H30" s="15">
+      <c r="H30" s="14">
         <v>0</v>
       </c>
-      <c r="I30" s="15">
+      <c r="I30" s="14">
         <v>0</v>
       </c>
-      <c r="J30" s="15">
+      <c r="J30" s="14">
         <v>0</v>
       </c>
-      <c r="K30" s="15">
+      <c r="K30" s="14">
         <v>0</v>
       </c>
-      <c r="L30" s="15">
+      <c r="L30" s="14">
         <v>1</v>
       </c>
-      <c r="M30" s="16">
+      <c r="M30" s="15">
         <v>0</v>
       </c>
       <c r="N30">
@@ -20961,502 +22277,502 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="21"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="19"/>
     </row>
     <row r="5" spans="3:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>2</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>3</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>4</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>5</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <v>6</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="2">
         <v>7</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="2">
         <v>8</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="2">
         <v>9</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>14</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>18</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>22</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <v>27</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="6">
         <v>23</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="6">
         <v>21</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="6">
         <v>27</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="6">
         <v>31</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="6">
         <v>20</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="7">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>22</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <v>20</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="10">
         <v>19</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="10">
         <v>19</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="10">
         <v>25</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="10">
         <v>19</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="10">
         <v>28</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="10">
         <v>20</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="10">
         <v>27</v>
       </c>
-      <c r="M7" s="12">
+      <c r="M7" s="11">
         <v>39</v>
       </c>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>12</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="10">
         <v>18</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <v>17</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="10">
         <v>16</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="10">
         <v>25</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="10">
         <v>30</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="10">
         <v>27</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="10">
         <v>26</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="10">
         <v>29</v>
       </c>
-      <c r="M8" s="12">
+      <c r="M8" s="11">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>12</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="10">
         <v>23</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="10">
         <v>26</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="10">
         <v>19</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="10">
         <v>26</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="10">
         <v>20</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="10">
         <v>26</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="10">
         <v>34</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="10">
         <v>23</v>
       </c>
-      <c r="M9" s="12">
+      <c r="M9" s="11">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>12</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="10">
         <v>14</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="10">
         <v>14</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="10">
         <v>19</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="10">
         <v>21</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="10">
         <v>27</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="10">
         <v>24</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="10">
         <v>28</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="10">
         <v>26</v>
       </c>
-      <c r="M10" s="12">
+      <c r="M10" s="11">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>20</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="10">
         <v>18</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="10">
         <v>20</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="10">
         <v>19</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="10">
         <v>15</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="10">
         <v>20</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="10">
         <v>31</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="10">
         <v>32</v>
       </c>
-      <c r="L11" s="11">
+      <c r="L11" s="10">
         <v>26</v>
       </c>
-      <c r="M11" s="12">
+      <c r="M11" s="11">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <v>15</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="10">
         <v>23</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="10">
         <v>20</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="10">
         <v>23</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="10">
         <v>26</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="10">
         <v>22</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="10">
         <v>32</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="10">
         <v>24</v>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="10">
         <v>26</v>
       </c>
-      <c r="M12" s="12">
+      <c r="M12" s="11">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <v>13</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="10">
         <v>14</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="10">
         <v>19</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="10">
         <v>20</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="10">
         <v>21</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="10">
         <v>22</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="10">
         <v>32</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="10">
         <v>24</v>
       </c>
-      <c r="L13" s="11">
+      <c r="L13" s="10">
         <v>31</v>
       </c>
-      <c r="M13" s="12">
+      <c r="M13" s="11">
         <v>29</v>
       </c>
     </row>
     <row r="14" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="9">
         <v>14</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="10">
         <v>19</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="10">
         <v>15</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="10">
         <v>16</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="10">
         <v>20</v>
       </c>
-      <c r="I14" s="11">
+      <c r="I14" s="10">
         <v>22</v>
       </c>
-      <c r="J14" s="11">
+      <c r="J14" s="10">
         <v>27</v>
       </c>
-      <c r="K14" s="11">
+      <c r="K14" s="10">
         <v>33</v>
       </c>
-      <c r="L14" s="11">
+      <c r="L14" s="10">
         <v>19</v>
       </c>
-      <c r="M14" s="12">
+      <c r="M14" s="11">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="3:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="13">
         <v>18</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="14">
         <v>23</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="14">
         <v>14</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G15" s="14">
         <v>23</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="14">
         <v>24</v>
       </c>
-      <c r="I15" s="15">
+      <c r="I15" s="14">
         <v>31</v>
       </c>
-      <c r="J15" s="15">
+      <c r="J15" s="14">
         <v>18</v>
       </c>
-      <c r="K15" s="15">
+      <c r="K15" s="14">
         <v>19</v>
       </c>
-      <c r="L15" s="15">
+      <c r="L15" s="14">
         <v>32</v>
       </c>
-      <c r="M15" s="16">
+      <c r="M15" s="15">
         <v>35</v>
       </c>
     </row>
     <row r="16" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
     </row>
     <row r="18" spans="3:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="3:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="21"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="19"/>
     </row>
     <row r="20" spans="3:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>1</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <v>2</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2">
         <v>3</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="2">
         <v>4</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="2">
         <v>5</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20" s="2">
         <v>6</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="2">
         <v>7</v>
       </c>
-      <c r="K20" s="3">
+      <c r="K20" s="2">
         <v>8</v>
       </c>
-      <c r="L20" s="3">
+      <c r="L20" s="2">
         <v>9</v>
       </c>
-      <c r="M20" s="4">
+      <c r="M20" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="5">
         <v>0</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="6">
         <v>0</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="6">
         <v>0</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="6">
         <v>0</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H21" s="6">
         <v>0</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="6">
         <v>0</v>
       </c>
-      <c r="J21" s="7">
+      <c r="J21" s="6">
         <v>0</v>
       </c>
-      <c r="K21" s="7">
+      <c r="K21" s="6">
         <v>0</v>
       </c>
-      <c r="L21" s="7">
+      <c r="L21" s="6">
         <v>0</v>
       </c>
-      <c r="M21" s="8">
+      <c r="M21" s="7">
         <v>1</v>
       </c>
       <c r="N21">
@@ -21465,37 +22781,37 @@
       </c>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="9">
         <v>0</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E22" s="10">
         <v>0</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="10">
         <v>0</v>
       </c>
-      <c r="G22" s="11">
+      <c r="G22" s="10">
         <v>0</v>
       </c>
-      <c r="H22" s="11">
+      <c r="H22" s="10">
         <v>0</v>
       </c>
-      <c r="I22" s="11">
+      <c r="I22" s="10">
         <v>0</v>
       </c>
-      <c r="J22" s="11">
+      <c r="J22" s="10">
         <v>0</v>
       </c>
-      <c r="K22" s="11">
+      <c r="K22" s="10">
         <v>1</v>
       </c>
-      <c r="L22" s="11">
+      <c r="L22" s="10">
         <v>0</v>
       </c>
-      <c r="M22" s="12">
+      <c r="M22" s="11">
         <v>0</v>
       </c>
       <c r="N22">
@@ -21504,37 +22820,37 @@
       </c>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="9">
         <v>0</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E23" s="10">
         <v>0</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="10">
         <v>0</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="10">
         <v>1</v>
       </c>
-      <c r="H23" s="11">
+      <c r="H23" s="10">
         <v>0</v>
       </c>
-      <c r="I23" s="11">
+      <c r="I23" s="10">
         <v>0</v>
       </c>
-      <c r="J23" s="11">
+      <c r="J23" s="10">
         <v>0</v>
       </c>
-      <c r="K23" s="11">
+      <c r="K23" s="10">
         <v>0</v>
       </c>
-      <c r="L23" s="11">
+      <c r="L23" s="10">
         <v>0</v>
       </c>
-      <c r="M23" s="12">
+      <c r="M23" s="11">
         <v>0</v>
       </c>
       <c r="N23">
@@ -21543,37 +22859,37 @@
       </c>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="9">
         <v>1</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="10">
         <v>0</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="10">
         <v>0</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G24" s="10">
         <v>0</v>
       </c>
-      <c r="H24" s="11">
+      <c r="H24" s="10">
         <v>0</v>
       </c>
-      <c r="I24" s="11">
+      <c r="I24" s="10">
         <v>0</v>
       </c>
-      <c r="J24" s="11">
+      <c r="J24" s="10">
         <v>0</v>
       </c>
-      <c r="K24" s="11">
+      <c r="K24" s="10">
         <v>0</v>
       </c>
-      <c r="L24" s="11">
+      <c r="L24" s="10">
         <v>0</v>
       </c>
-      <c r="M24" s="12">
+      <c r="M24" s="11">
         <v>0</v>
       </c>
       <c r="N24">
@@ -21582,37 +22898,37 @@
       </c>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="9">
         <v>0</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="10">
         <v>0</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="10">
         <v>1</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G25" s="10">
         <v>0</v>
       </c>
-      <c r="H25" s="11">
+      <c r="H25" s="10">
         <v>0</v>
       </c>
-      <c r="I25" s="11">
+      <c r="I25" s="10">
         <v>0</v>
       </c>
-      <c r="J25" s="11">
+      <c r="J25" s="10">
         <v>0</v>
       </c>
-      <c r="K25" s="11">
+      <c r="K25" s="10">
         <v>0</v>
       </c>
-      <c r="L25" s="11">
+      <c r="L25" s="10">
         <v>0</v>
       </c>
-      <c r="M25" s="12">
+      <c r="M25" s="11">
         <v>0</v>
       </c>
       <c r="N25">
@@ -21621,37 +22937,37 @@
       </c>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="9">
         <v>0</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26" s="10">
         <v>0</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="10">
         <v>0</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G26" s="10">
         <v>0</v>
       </c>
-      <c r="H26" s="11">
+      <c r="H26" s="10">
         <v>1</v>
       </c>
-      <c r="I26" s="11">
+      <c r="I26" s="10">
         <v>0</v>
       </c>
-      <c r="J26" s="11">
+      <c r="J26" s="10">
         <v>0</v>
       </c>
-      <c r="K26" s="11">
+      <c r="K26" s="10">
         <v>0</v>
       </c>
-      <c r="L26" s="11">
+      <c r="L26" s="10">
         <v>0</v>
       </c>
-      <c r="M26" s="12">
+      <c r="M26" s="11">
         <v>0</v>
       </c>
       <c r="N26">
@@ -21660,37 +22976,37 @@
       </c>
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27" s="9">
         <v>0</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E27" s="10">
         <v>0</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F27" s="10">
         <v>0</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G27" s="10">
         <v>0</v>
       </c>
-      <c r="H27" s="11">
+      <c r="H27" s="10">
         <v>0</v>
       </c>
-      <c r="I27" s="11">
+      <c r="I27" s="10">
         <v>1</v>
       </c>
-      <c r="J27" s="11">
+      <c r="J27" s="10">
         <v>0</v>
       </c>
-      <c r="K27" s="11">
+      <c r="K27" s="10">
         <v>0</v>
       </c>
-      <c r="L27" s="11">
+      <c r="L27" s="10">
         <v>0</v>
       </c>
-      <c r="M27" s="12">
+      <c r="M27" s="11">
         <v>0</v>
       </c>
       <c r="N27">
@@ -21699,37 +23015,37 @@
       </c>
     </row>
     <row r="28" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="9">
         <v>0</v>
       </c>
-      <c r="E28" s="11">
+      <c r="E28" s="10">
         <v>1</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F28" s="10">
         <v>0</v>
       </c>
-      <c r="G28" s="11">
+      <c r="G28" s="10">
         <v>0</v>
       </c>
-      <c r="H28" s="11">
+      <c r="H28" s="10">
         <v>0</v>
       </c>
-      <c r="I28" s="11">
+      <c r="I28" s="10">
         <v>0</v>
       </c>
-      <c r="J28" s="11">
+      <c r="J28" s="10">
         <v>0</v>
       </c>
-      <c r="K28" s="11">
+      <c r="K28" s="10">
         <v>0</v>
       </c>
-      <c r="L28" s="11">
+      <c r="L28" s="10">
         <v>0</v>
       </c>
-      <c r="M28" s="12">
+      <c r="M28" s="11">
         <v>0</v>
       </c>
       <c r="N28">
@@ -21738,37 +23054,37 @@
       </c>
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="9">
         <v>0</v>
       </c>
-      <c r="E29" s="11">
+      <c r="E29" s="10">
         <v>0</v>
       </c>
-      <c r="F29" s="11">
+      <c r="F29" s="10">
         <v>0</v>
       </c>
-      <c r="G29" s="11">
+      <c r="G29" s="10">
         <v>0</v>
       </c>
-      <c r="H29" s="11">
+      <c r="H29" s="10">
         <v>0</v>
       </c>
-      <c r="I29" s="11">
+      <c r="I29" s="10">
         <v>0</v>
       </c>
-      <c r="J29" s="11">
+      <c r="J29" s="10">
         <v>0</v>
       </c>
-      <c r="K29" s="11">
+      <c r="K29" s="10">
         <v>0</v>
       </c>
-      <c r="L29" s="11">
+      <c r="L29" s="10">
         <v>1</v>
       </c>
-      <c r="M29" s="12">
+      <c r="M29" s="11">
         <v>0</v>
       </c>
       <c r="N29">
@@ -21777,37 +23093,37 @@
       </c>
     </row>
     <row r="30" spans="3:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="14">
+      <c r="D30" s="13">
         <v>0</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="14">
         <v>0</v>
       </c>
-      <c r="F30" s="15">
+      <c r="F30" s="14">
         <v>0</v>
       </c>
-      <c r="G30" s="15">
+      <c r="G30" s="14">
         <v>0</v>
       </c>
-      <c r="H30" s="15">
+      <c r="H30" s="14">
         <v>0</v>
       </c>
-      <c r="I30" s="15">
+      <c r="I30" s="14">
         <v>0</v>
       </c>
-      <c r="J30" s="15">
+      <c r="J30" s="14">
         <v>1</v>
       </c>
-      <c r="K30" s="15">
+      <c r="K30" s="14">
         <v>0</v>
       </c>
-      <c r="L30" s="15">
+      <c r="L30" s="14">
         <v>0</v>
       </c>
-      <c r="M30" s="16">
+      <c r="M30" s="15">
         <v>0</v>
       </c>
       <c r="N30">
@@ -21873,339 +23189,615 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="B4:G19"/>
+  <dimension ref="B3:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="18" t="s">
+    <row r="3" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B4" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="D4" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="E4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="C5" s="24">
+        <v>2.15</v>
+      </c>
+      <c r="D5" s="24">
+        <v>2.27</v>
+      </c>
+      <c r="E5" s="25">
+        <v>300</v>
+      </c>
+      <c r="F5" s="25">
+        <v>1500</v>
+      </c>
+      <c r="G5" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="H5" s="25">
+        <v>300</v>
+      </c>
+      <c r="I5" s="32">
+        <f>H5*G5</f>
+        <v>375</v>
+      </c>
+      <c r="J5" s="36">
+        <f>C5*$H5</f>
+        <v>645</v>
+      </c>
+      <c r="K5" s="37">
+        <f>D5*$H5</f>
+        <v>681</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="24">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D6" s="24">
+        <v>2.48</v>
+      </c>
+      <c r="E6" s="25">
+        <v>400</v>
+      </c>
+      <c r="F6" s="25">
+        <v>2000</v>
+      </c>
+      <c r="G6" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="H6" s="25">
+        <v>2000</v>
+      </c>
+      <c r="I6" s="32">
+        <f t="shared" ref="I6:I19" si="0">H6*G6</f>
+        <v>2500</v>
+      </c>
+      <c r="J6" s="36">
+        <f t="shared" ref="J6:J18" si="1">C6*$H6</f>
+        <v>4400</v>
+      </c>
+      <c r="K6" s="37">
+        <f t="shared" ref="K6:K18" si="2">D6*$H6</f>
+        <v>4960</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="24">
+        <v>2.4</v>
+      </c>
+      <c r="D7" s="24">
+        <v>2.7</v>
+      </c>
+      <c r="E7" s="25">
+        <v>250</v>
+      </c>
+      <c r="F7" s="25">
+        <v>900</v>
+      </c>
+      <c r="G7" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="H7" s="25">
+        <v>900</v>
+      </c>
+      <c r="I7" s="32">
+        <f t="shared" si="0"/>
+        <v>1125</v>
+      </c>
+      <c r="J7" s="36">
+        <f t="shared" si="1"/>
+        <v>2160</v>
+      </c>
+      <c r="K7" s="37">
+        <f t="shared" si="2"/>
+        <v>2430</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="24">
+        <v>4.8</v>
+      </c>
+      <c r="D8" s="24">
+        <v>5.2</v>
+      </c>
+      <c r="E8" s="25">
         <v>0</v>
       </c>
-      <c r="F4" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>33</v>
+      <c r="F8" s="25">
+        <v>150</v>
+      </c>
+      <c r="G8" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="H8" s="25">
+        <v>0</v>
+      </c>
+      <c r="I8" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="37">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2.15</v>
-      </c>
-      <c r="D5" s="1">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B9" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="24">
+        <v>2.6</v>
+      </c>
+      <c r="D9" s="24">
+        <v>2.92</v>
+      </c>
+      <c r="E9" s="25">
+        <v>300</v>
+      </c>
+      <c r="F9" s="25">
+        <v>1200</v>
+      </c>
+      <c r="G9" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="H9" s="25">
+        <v>1200</v>
+      </c>
+      <c r="I9" s="32">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="J9" s="36">
+        <f t="shared" si="1"/>
+        <v>3120</v>
+      </c>
+      <c r="K9" s="37">
+        <f t="shared" si="2"/>
+        <v>3504</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="24">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D10" s="24">
+        <v>2.48</v>
+      </c>
+      <c r="E10" s="25">
+        <v>200</v>
+      </c>
+      <c r="F10" s="25">
+        <v>800</v>
+      </c>
+      <c r="G10" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="H10" s="25">
+        <v>200</v>
+      </c>
+      <c r="I10" s="32">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+      <c r="J10" s="36">
+        <f t="shared" si="1"/>
+        <v>459.99999999999994</v>
+      </c>
+      <c r="K10" s="37">
+        <f t="shared" si="2"/>
+        <v>496</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B11" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="24">
+        <v>2.35</v>
+      </c>
+      <c r="D11" s="24">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E11" s="25">
+        <v>150</v>
+      </c>
+      <c r="F11" s="25">
+        <v>600</v>
+      </c>
+      <c r="G11" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="H11" s="25">
+        <v>150</v>
+      </c>
+      <c r="I11" s="32">
+        <f t="shared" si="0"/>
+        <v>187.5</v>
+      </c>
+      <c r="J11" s="36">
+        <f t="shared" si="1"/>
+        <v>352.5</v>
+      </c>
+      <c r="K11" s="37">
+        <f t="shared" si="2"/>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="24">
+        <v>2.85</v>
+      </c>
+      <c r="D12" s="24">
+        <v>3.13</v>
+      </c>
+      <c r="E12" s="25">
+        <v>100</v>
+      </c>
+      <c r="F12" s="25">
+        <v>300</v>
+      </c>
+      <c r="G12" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="H12" s="25">
+        <v>100</v>
+      </c>
+      <c r="I12" s="32">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+      <c r="J12" s="36">
+        <f t="shared" si="1"/>
+        <v>285</v>
+      </c>
+      <c r="K12" s="37">
+        <f t="shared" si="2"/>
+        <v>313</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B13" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="24">
+        <v>2.25</v>
+      </c>
+      <c r="D13" s="24">
+        <v>2.48</v>
+      </c>
+      <c r="E13" s="25">
+        <v>750</v>
+      </c>
+      <c r="F13" s="25">
+        <v>3500</v>
+      </c>
+      <c r="G13" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="H13" s="25">
+        <v>750</v>
+      </c>
+      <c r="I13" s="32">
+        <f t="shared" si="0"/>
+        <v>937.5</v>
+      </c>
+      <c r="J13" s="36">
+        <f t="shared" si="1"/>
+        <v>1687.5</v>
+      </c>
+      <c r="K13" s="37">
+        <f t="shared" si="2"/>
+        <v>1860</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B14" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="24">
+        <v>2.1</v>
+      </c>
+      <c r="D14" s="24">
         <v>2.27</v>
       </c>
-      <c r="E5">
+      <c r="E14" s="25">
+        <v>400</v>
+      </c>
+      <c r="F14" s="25">
+        <v>2000</v>
+      </c>
+      <c r="G14" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="H14" s="25">
+        <v>400</v>
+      </c>
+      <c r="I14" s="32">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="J14" s="36">
+        <f t="shared" si="1"/>
+        <v>840</v>
+      </c>
+      <c r="K14" s="37">
+        <f t="shared" si="2"/>
+        <v>908</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B15" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="24">
+        <v>2.8</v>
+      </c>
+      <c r="D15" s="24">
+        <v>3.13</v>
+      </c>
+      <c r="E15" s="25">
+        <v>500</v>
+      </c>
+      <c r="F15" s="25">
+        <v>3300</v>
+      </c>
+      <c r="G15" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="H15" s="25">
+        <v>2150</v>
+      </c>
+      <c r="I15" s="32">
+        <f t="shared" si="0"/>
+        <v>2687.5</v>
+      </c>
+      <c r="J15" s="36">
+        <f t="shared" si="1"/>
+        <v>6020</v>
+      </c>
+      <c r="K15" s="37">
+        <f t="shared" si="2"/>
+        <v>6729.5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="24">
+        <v>3</v>
+      </c>
+      <c r="D16" s="24">
+        <v>3.18</v>
+      </c>
+      <c r="E16" s="25">
+        <v>100</v>
+      </c>
+      <c r="F16" s="25">
+        <v>500</v>
+      </c>
+      <c r="G16" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="H16" s="25">
+        <v>100</v>
+      </c>
+      <c r="I16" s="32">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+      <c r="J16" s="36">
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
-      <c r="F5">
-        <v>1500</v>
-      </c>
-      <c r="G5">
+      <c r="K16" s="37">
+        <f t="shared" si="2"/>
+        <v>318</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B17" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="24">
+        <v>2.6</v>
+      </c>
+      <c r="D17" s="24">
+        <v>2.92</v>
+      </c>
+      <c r="E17" s="25">
+        <v>500</v>
+      </c>
+      <c r="F17" s="25">
+        <v>3200</v>
+      </c>
+      <c r="G17" s="25">
         <v>1.25</v>
       </c>
+      <c r="H17" s="25">
+        <v>3200</v>
+      </c>
+      <c r="I17" s="32">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+      <c r="J17" s="36">
+        <f t="shared" si="1"/>
+        <v>8320</v>
+      </c>
+      <c r="K17" s="37">
+        <f t="shared" si="2"/>
+        <v>9344</v>
+      </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2.48</v>
-      </c>
-      <c r="E6">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B18" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="24">
+        <v>2.5</v>
+      </c>
+      <c r="D18" s="24">
+        <v>2.7</v>
+      </c>
+      <c r="E18" s="25">
+        <v>100</v>
+      </c>
+      <c r="F18" s="25">
+        <v>500</v>
+      </c>
+      <c r="G18" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="H18" s="25">
+        <v>100</v>
+      </c>
+      <c r="I18" s="32">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+      <c r="J18" s="36">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+      <c r="K18" s="37">
+        <f t="shared" si="2"/>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="27">
+        <v>2.9</v>
+      </c>
+      <c r="D19" s="27">
+        <v>3.13</v>
+      </c>
+      <c r="E19" s="28">
         <v>400</v>
       </c>
-      <c r="F6">
-        <v>2000</v>
-      </c>
-      <c r="G6">
+      <c r="F19" s="28">
+        <v>2500</v>
+      </c>
+      <c r="G19" s="28">
         <v>1.25</v>
       </c>
+      <c r="H19" s="25">
+        <v>400</v>
+      </c>
+      <c r="I19" s="32">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="J19" s="36">
+        <f>C19*$H19</f>
+        <v>1160</v>
+      </c>
+      <c r="K19" s="37">
+        <f>D19*$H19</f>
+        <v>1252</v>
+      </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1">
-        <v>2.4</v>
-      </c>
-      <c r="D7" s="1">
-        <v>2.7</v>
-      </c>
-      <c r="E7">
-        <v>250</v>
-      </c>
-      <c r="F7">
-        <v>900</v>
-      </c>
-      <c r="G7">
-        <v>1.25</v>
+    <row r="20" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="33">
+        <f>SUM(I5:I19)</f>
+        <v>14937.5</v>
+      </c>
+      <c r="J20" s="33">
+        <f>SUM(J5:J19)</f>
+        <v>30000</v>
+      </c>
+      <c r="K20" s="38">
+        <f>SUM(K5:K19)</f>
+        <v>33395.5</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="1">
-        <v>4.8</v>
-      </c>
-      <c r="D8" s="1">
-        <v>5.2</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>150</v>
-      </c>
-      <c r="G8">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2.6</v>
-      </c>
-      <c r="D9" s="1">
-        <v>2.92</v>
-      </c>
-      <c r="E9">
-        <v>300</v>
-      </c>
-      <c r="F9">
-        <v>1200</v>
-      </c>
-      <c r="G9">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="1">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D10" s="1">
-        <v>2.48</v>
-      </c>
-      <c r="E10">
-        <v>200</v>
-      </c>
-      <c r="F10">
-        <v>800</v>
-      </c>
-      <c r="G10">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="1">
-        <v>2.35</v>
-      </c>
-      <c r="D11" s="1">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E11">
-        <v>150</v>
-      </c>
-      <c r="F11">
-        <v>600</v>
-      </c>
-      <c r="G11">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2.85</v>
-      </c>
-      <c r="D12" s="1">
-        <v>3.13</v>
-      </c>
-      <c r="E12">
-        <v>100</v>
-      </c>
-      <c r="F12">
-        <v>300</v>
-      </c>
-      <c r="G12">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="1">
-        <v>2.25</v>
-      </c>
-      <c r="D13" s="1">
-        <v>2.48</v>
-      </c>
-      <c r="E13">
-        <v>750</v>
-      </c>
-      <c r="F13">
-        <v>3500</v>
-      </c>
-      <c r="G13">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="1">
-        <v>2.1</v>
-      </c>
-      <c r="D14" s="1">
-        <v>2.27</v>
-      </c>
-      <c r="E14">
-        <v>400</v>
-      </c>
-      <c r="F14">
-        <v>2000</v>
-      </c>
-      <c r="G14">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="1">
-        <v>2.8</v>
-      </c>
-      <c r="D15" s="1">
-        <v>3.13</v>
-      </c>
-      <c r="E15">
-        <v>500</v>
-      </c>
-      <c r="F15">
-        <v>3300</v>
-      </c>
-      <c r="G15">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="1">
-        <v>3</v>
-      </c>
-      <c r="D16" s="1">
-        <v>3.18</v>
-      </c>
-      <c r="E16">
-        <v>100</v>
-      </c>
-      <c r="F16">
-        <v>500</v>
-      </c>
-      <c r="G16">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="1">
-        <v>2.6</v>
-      </c>
-      <c r="D17" s="1">
-        <v>2.92</v>
-      </c>
-      <c r="E17">
-        <v>500</v>
-      </c>
-      <c r="F17">
-        <v>3200</v>
-      </c>
-      <c r="G17">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="D18" s="1">
-        <v>2.7</v>
-      </c>
-      <c r="E18">
-        <v>100</v>
-      </c>
-      <c r="F18">
-        <v>500</v>
-      </c>
-      <c r="G18">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="1">
-        <v>2.9</v>
-      </c>
-      <c r="D19" s="1">
-        <v>3.13</v>
-      </c>
-      <c r="E19">
-        <v>400</v>
-      </c>
-      <c r="F19">
-        <v>2500</v>
-      </c>
-      <c r="G19">
-        <v>1.25</v>
+    <row r="21" spans="2:13" ht="24" x14ac:dyDescent="0.3">
+      <c r="L21" s="34">
+        <f>K20-J20</f>
+        <v>3395.5</v>
+      </c>
+      <c r="M21" s="35" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>